<commit_message>
added extra sheets in spreadsheet
</commit_message>
<xml_diff>
--- a/code/instAlgoMatrix_60.xlsx
+++ b/code/instAlgoMatrix_60.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="optValues" r:id="rId2" sheetId="1" state="visible"/>
-    <sheet name="runningTimes" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="firstLB" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="numberNodes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="optValues" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="runningTimes" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="27">
   <si>
     <t xml:space="preserve">Instances</t>
   </si>
@@ -102,57 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">rbg443</t>
-  </si>
-  <si>
-    <t>39.0</t>
-  </si>
-  <si>
-    <t>3.169E-6</t>
-  </si>
-  <si>
-    <t>2.849E-6</t>
-  </si>
-  <si>
-    <t>3.594E-6</t>
-  </si>
-  <si>
-    <t>2.996E-6</t>
-  </si>
-  <si>
-    <t>38673.0</t>
-  </si>
-  <si>
-    <t>3.466E-6</t>
-  </si>
-  <si>
-    <t>2.742E-6</t>
-  </si>
-  <si>
-    <t>3.735E-6</t>
-  </si>
-  <si>
-    <t>3.905E-6</t>
-  </si>
-  <si>
-    <t>3.568E-6</t>
-  </si>
-  <si>
-    <t>2.937E-6</t>
-  </si>
-  <si>
-    <t>3.179E-6</t>
-  </si>
-  <si>
-    <t>3.137E-6</t>
-  </si>
-  <si>
-    <t>3.714E-6</t>
-  </si>
-  <si>
-    <t>3.372E-6</t>
-  </si>
-  <si>
-    <t>2.913E-6</t>
   </si>
 </sst>
 </file>
@@ -194,7 +145,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -203,68 +154,69 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1023" max="1024" customWidth="true" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -290,120 +242,105 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="15">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -412,22 +349,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C24" activeCellId="0" pane="topLeft" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1023" max="1024" customWidth="true" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,120 +391,403 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="15">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="19">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>